<commit_message>
3V3 LDO replaced, reverse polarity bug fixed
</commit_message>
<xml_diff>
--- a/STM32G031_SOIC8_Dev_Board/Project Outputs for STM32G031_SOIC8_Dev_Board/STM32G031_SOIC8_Dev_Board_rev_1.0.xlsx
+++ b/STM32G031_SOIC8_Dev_Board/Project Outputs for STM32G031_SOIC8_Dev_Board/STM32G031_SOIC8_Dev_Board_rev_1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\javi_\GitHub\STM32G031_SOIC8_Dev_Board\2022_03_17_STM32G031_SOIC8_Dev_Board\Project Outputs for STM32G031_SOIC8_Dev_Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javi_\GitHub\STM32G031_SOIC8_Dev_Board\STM32G031_SOIC8_Dev_Board\Project Outputs for STM32G031_SOIC8_Dev_Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC386F50-CFF5-4AAC-B1F0-1FCCDECA2999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8A1BF6A-54F9-41B1-B075-4B4CCFE9786B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17580" yWindow="2175" windowWidth="17355" windowHeight="17865" xr2:uid="{A2BFBC63-71A8-4E92-9E50-B446CF3A6307}"/>
+    <workbookView xWindow="9255" yWindow="930" windowWidth="23550" windowHeight="16410" xr2:uid="{ECEA07BA-C292-42DE-8E18-F80B594C5E5A}"/>
   </bookViews>
   <sheets>
     <sheet name="STM32G031_SOIC8_Dev_Board_rev_1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
   <si>
     <t>Comment</t>
   </si>
@@ -112,13 +112,13 @@
     <t>CN2, CN6</t>
   </si>
   <si>
-    <t>CN_8PIN</t>
+    <t>CN_10PIN</t>
   </si>
   <si>
     <t>CN4, CN5</t>
   </si>
   <si>
-    <t>920-E52A2021S10100</t>
+    <t>USB_B_AE</t>
   </si>
   <si>
     <t>USB connector</t>
@@ -127,10 +127,7 @@
     <t>CN7</t>
   </si>
   <si>
-    <t>USB307530A</t>
-  </si>
-  <si>
-    <t>BAT54C_R1_00001</t>
+    <t>RB715UMTL</t>
   </si>
   <si>
     <t>Schottky Diode</t>
@@ -139,7 +136,7 @@
     <t>D1</t>
   </si>
   <si>
-    <t>SOT95P240X110-3N</t>
+    <t>DAN217UMTL</t>
   </si>
   <si>
     <t>STM32G031J6M6</t>
@@ -154,19 +151,22 @@
     <t>SOIC127P600X175-8N</t>
   </si>
   <si>
-    <t>NCP115ASN330T2G</t>
+    <t>MIC5366-3.3YC5-TR</t>
+  </si>
+  <si>
+    <t>LDO</t>
   </si>
   <si>
     <t>IC2</t>
   </si>
   <si>
-    <t>3.3V/300mA</t>
-  </si>
-  <si>
-    <t>SOT95P275X110-5N</t>
-  </si>
-  <si>
-    <t>MIC5365-1.8YD5-TR</t>
+    <t>3.3V/150mA</t>
+  </si>
+  <si>
+    <t>SOT65P210X110-5N</t>
+  </si>
+  <si>
+    <t>AP2120N-1.8TRG1</t>
   </si>
   <si>
     <t>IC3</t>
@@ -175,7 +175,10 @@
     <t>1.8V/150mA</t>
   </si>
   <si>
-    <t>150080YS75000_Y</t>
+    <t>SOT95P230X110-3N</t>
+  </si>
+  <si>
+    <t>LTST-C171KSKT</t>
   </si>
   <si>
     <t>LED</t>
@@ -184,19 +187,19 @@
     <t>LD1</t>
   </si>
   <si>
-    <t>Yellow</t>
+    <t>Yellow/20mA</t>
   </si>
   <si>
     <t>LEDC2012X85N_Y</t>
   </si>
   <si>
-    <t>150080VS75000_G</t>
+    <t>LTST-C171KGKT</t>
   </si>
   <si>
     <t>LD2</t>
   </si>
   <si>
-    <t>Green</t>
+    <t>Green/20mA</t>
   </si>
   <si>
     <t>LEDC2012X85N_G</t>
@@ -217,6 +220,18 @@
     <t>RESC2012X60N</t>
   </si>
   <si>
+    <t>PTS815_SJM_250_SMTR_LFS</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>PTS815SJM250SMTRLFS</t>
+  </si>
+  <si>
     <t>RC0805FR-070RL</t>
   </si>
   <si>
@@ -224,15 +239,6 @@
   </si>
   <si>
     <t>SB1</t>
-  </si>
-  <si>
-    <t>EVP-BT3G4A000</t>
-  </si>
-  <si>
-    <t>Tactile switch</t>
-  </si>
-  <si>
-    <t>SW1</t>
   </si>
   <si>
     <t>ASEKDV-32.768kHz-LC-T</t>
@@ -620,7 +626,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A43724-94BF-4831-9B1C-CF654DAE657D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341F517A-078E-4E55-9F1B-4FA50280A572}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -806,57 +812,57 @@
         <v>26</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>39</v>
@@ -868,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>41</v>
@@ -879,7 +885,7 @@
         <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>43</v>
@@ -894,141 +900,141 @@
         <v>42</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="G18" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>